<commit_message>
Sun May  3 07:38:45 IST 2020
</commit_message>
<xml_diff>
--- a/output/reports/03-parsed-network-configs.xlsx
+++ b/output/reports/03-parsed-network-configs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="189">
   <si>
     <t>TCL NETWORK ASSESSMENT - [M3] WAN NETWORK DEVICE CONFIGURATION PARSER MODULE</t>
   </si>
@@ -380,6 +380,192 @@
   </si>
   <si>
     <t>vrf forwarding Mgmt-intf</t>
+  </si>
+  <si>
+    <t>Routing Context</t>
+  </si>
+  <si>
+    <t>OSPF</t>
+  </si>
+  <si>
+    <t>router ospf 1 vrf NC1</t>
+  </si>
+  <si>
+    <t>capability vrf-lite</t>
+  </si>
+  <si>
+    <t>area 10.168.224.32 nssa</t>
+  </si>
+  <si>
+    <t>redistribute bgp 64982 metric 1000 metric-type 1 subnets route-map NC1</t>
+  </si>
+  <si>
+    <t>network 10.168.224.189 0.0.0.0 area 10.168.224.32</t>
+  </si>
+  <si>
+    <t>distribute-list 1 out</t>
+  </si>
+  <si>
+    <t>BGP</t>
+  </si>
+  <si>
+    <t>router bgp 64982</t>
+  </si>
+  <si>
+    <t>bgp router-id 172.23.32.11</t>
+  </si>
+  <si>
+    <t>bgp log-neighbor-changes</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>address-family ipv4 vrf NC1</t>
+  </si>
+  <si>
+    <t>exit-address-family</t>
+  </si>
+  <si>
+    <t>address-family ipv4 vrf NC3</t>
+  </si>
+  <si>
+    <t>EIGRP</t>
+  </si>
+  <si>
+    <t>RIP</t>
+  </si>
+  <si>
+    <t>STATIC</t>
+  </si>
+  <si>
+    <t>ip route vrf NC3 0.0.0.0 0.0.0.0 10.168.224.51</t>
+  </si>
+  <si>
+    <t>Router Filters &amp; Manipulations</t>
+  </si>
+  <si>
+    <t>Route-Map</t>
+  </si>
+  <si>
+    <t>route-map TCL_eBGP_OUT deny 10</t>
+  </si>
+  <si>
+    <t>match as-path 100</t>
+  </si>
+  <si>
+    <t>route-map TCL_eBGP_OUT deny 15</t>
+  </si>
+  <si>
+    <t>match ip address prefix-list BOSCH_MON</t>
+  </si>
+  <si>
+    <t>route-map TCL_eBGP_OUT permit 20</t>
+  </si>
+  <si>
+    <t>route-map TCL_eBGP deny 10</t>
+  </si>
+  <si>
+    <t>route-map TCL_eBGP deny 15</t>
+  </si>
+  <si>
+    <t>route-map TCL_eBGP permit 20</t>
+  </si>
+  <si>
+    <t>route-map NC1 permit 10</t>
+  </si>
+  <si>
+    <t>match ip address prefix-list NC1-WAN</t>
+  </si>
+  <si>
+    <t>route-map HS_DEFAULT_ROUTE_DENY deny 10</t>
+  </si>
+  <si>
+    <t>match ip address prefix-list DEFAULT_ROUTE</t>
+  </si>
+  <si>
+    <t>route-map HS_DEFAULT_ROUTE_DENY permit 20</t>
+  </si>
+  <si>
+    <t>match ip address prefix-list HS_SUBCA2_SEC_KS</t>
+  </si>
+  <si>
+    <t>set local-preference 500</t>
+  </si>
+  <si>
+    <t>route-map HS_DEFAULT_ROUTE_DENY permit 30</t>
+  </si>
+  <si>
+    <t>route-map FM_DEFAULT_ROUTE_DENY deny 10</t>
+  </si>
+  <si>
+    <t>route-map FM_DEFAULT_ROUTE_DENY permit 20</t>
+  </si>
+  <si>
+    <t>match ip address prefix-list FM_SUBCA2_SEC_KS</t>
+  </si>
+  <si>
+    <t>route-map FM_DEFAULT_ROUTE_DENY permit 30</t>
+  </si>
+  <si>
+    <t>route-map SPECIFIC_ROUTES permit 10</t>
+  </si>
+  <si>
+    <t>match ip address prefix-list SPECIFIC_ROUTES</t>
+  </si>
+  <si>
+    <t>Prefix-List</t>
+  </si>
+  <si>
+    <t>ip prefix-list BOSCH_MON seq 10 permit 172.23.33.52/30 le 32</t>
+  </si>
+  <si>
+    <t>ip prefix-list DEFAULT_ROUTE seq 10 permit 0.0.0.0/0</t>
+  </si>
+  <si>
+    <t>ip prefix-list FM_SUBCA2_SEC_KS seq 10 permit 172.23.33.34/32</t>
+  </si>
+  <si>
+    <t>ip prefix-list FM_SUBCA2_SEC_KS seq 20 permit 172.23.33.36/32</t>
+  </si>
+  <si>
+    <t>ip prefix-list HS_SUBCA2_SEC_KS seq 10 permit 172.23.33.34/32</t>
+  </si>
+  <si>
+    <t>ip prefix-list HS_SUBCA2_SEC_KS seq 20 permit 172.23.33.37/32</t>
+  </si>
+  <si>
+    <t>ip prefix-list NC1-WAN seq 4 deny 10.124.0.0/16 le 32</t>
+  </si>
+  <si>
+    <t>ip prefix-list NC1-WAN seq 5 deny 0.0.0.0/0</t>
+  </si>
+  <si>
+    <t>ip prefix-list NC1-WAN seq 6 deny 172.23.33.32/28 le 32</t>
+  </si>
+  <si>
+    <t>ip prefix-list NC1-WAN seq 7 deny 10.75.0.0/16 le 32</t>
+  </si>
+  <si>
+    <t>ip prefix-list NC1-WAN seq 8 deny 10.77.0.0/16 le 32</t>
+  </si>
+  <si>
+    <t>ip prefix-list NC1-WAN seq 9 deny 10.95.0.0/16 le 32</t>
+  </si>
+  <si>
+    <t>ip prefix-list NC1-WAN seq 10 permit 0.0.0.0/0 ge 1</t>
+  </si>
+  <si>
+    <t>ip prefix-list SPECIFIC_ROUTES seq 10 deny 0.0.0.0/0</t>
+  </si>
+  <si>
+    <t>ip prefix-list SPECIFIC_ROUTES seq 20 permit 0.0.0.0/0 ge 29</t>
+  </si>
+  <si>
+    <t>ip prefix-list no-default-route seq 5 deny 0.0.0.0/0</t>
+  </si>
+  <si>
+    <t>ip prefix-list no-default-route seq 10 permit 0.0.0.0/0 ge 1</t>
   </si>
   <si>
     <t>192.168.0.109</t>
@@ -872,10 +1058,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>120</v>
+        <v>182</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>121</v>
+        <v>183</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
@@ -887,7 +1073,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>122</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -895,10 +1081,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>124</v>
+        <v>186</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
@@ -954,6 +1140,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="75.7109375" customWidth="1"/>
+    <col min="2" max="2" width="75.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -991,11 +1179,23 @@
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="5" t="s">
@@ -1006,383 +1206,585 @@
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="B9" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="B10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="B11" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="B12" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="B13" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="B14" s="5" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="C15" s="5" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="17" spans="1:3">
+      <c r="B17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="C18" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B22" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="C28" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="C29" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="C31" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="C32" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="C33" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B34" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="C35" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:3">
       <c r="A37" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="C37" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:3">
       <c r="A40" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="C41" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="C42" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:3">
       <c r="A44" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="C44" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:3">
       <c r="A46" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="C46" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="C47" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:3">
       <c r="A49" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:3">
       <c r="A50" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:3">
       <c r="A51" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="C51" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:3">
       <c r="A53" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="C53" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="C55" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:3">
       <c r="A57" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="C57" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:3">
       <c r="A59" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="C59" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="C61" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:3">
       <c r="A63" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="C63" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:3">
       <c r="A65" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="C65" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="C67" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:3">
       <c r="A69" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="C69" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:3">
       <c r="A71" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="C71" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="C73" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:3">
       <c r="A75" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="C75" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:3">
       <c r="A77" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="C77" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="C79" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:3">
       <c r="A81" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="C81" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:3">
       <c r="A83" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="C83" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:3">
       <c r="A85" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="C85" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:3">
       <c r="A87" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:3">
       <c r="A88" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:3">
       <c r="A89" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:3">
       <c r="A90" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:3">
       <c r="A92" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:3">
       <c r="A93" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:3">
       <c r="A94" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:3">
       <c r="A95" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:3">
       <c r="A96" s="5" t="s">
         <v>25</v>
       </c>
@@ -1915,6 +2317,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="75.7109375" customWidth="1"/>
+    <col min="2" max="2" width="75.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1925,7 +2329,7 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>123</v>
+        <v>185</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1952,11 +2356,23 @@
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="5" t="s">
@@ -1967,383 +2383,585 @@
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="B9" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="B10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="B11" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="B12" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="B13" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="B14" s="5" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="C15" s="5" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="17" spans="1:3">
+      <c r="B17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="C18" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B22" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="C28" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="C29" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="C31" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="C32" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="C33" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B34" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="C35" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:3">
       <c r="A37" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="C37" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:3">
       <c r="A40" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="C41" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="C42" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:3">
       <c r="A44" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="C44" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:3">
       <c r="A46" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="C46" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="C47" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:3">
       <c r="A49" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:3">
       <c r="A50" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:3">
       <c r="A51" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="C51" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:3">
       <c r="A53" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="C53" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="C55" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:3">
       <c r="A57" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="C57" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:3">
       <c r="A59" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="C59" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="C61" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:3">
       <c r="A63" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="C63" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:3">
       <c r="A65" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="C65" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="C67" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:3">
       <c r="A69" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="C69" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:3">
       <c r="A71" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="C71" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="C73" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:3">
       <c r="A75" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="C75" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:3">
       <c r="A77" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="C77" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="C79" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:3">
       <c r="A81" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="C81" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:3">
       <c r="A83" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="C83" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:3">
       <c r="A85" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="C85" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:3">
       <c r="A87" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:3">
       <c r="A88" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:3">
       <c r="A89" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:3">
       <c r="A90" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:3">
       <c r="A92" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:3">
       <c r="A93" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:3">
       <c r="A94" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:3">
       <c r="A95" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:3">
       <c r="A96" s="5" t="s">
         <v>25</v>
       </c>
@@ -2876,6 +3494,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="75.7109375" customWidth="1"/>
+    <col min="2" max="2" width="75.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2886,7 +3506,7 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>126</v>
+        <v>188</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2913,11 +3533,23 @@
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="5" t="s">
@@ -2928,383 +3560,585 @@
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="B9" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="B10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="B11" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="B12" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="B13" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="B14" s="5" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="C15" s="5" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="17" spans="1:3">
+      <c r="B17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="C18" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B22" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="C28" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="C29" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="C31" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="C32" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="C33" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B34" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="C35" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:3">
       <c r="A37" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="C37" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:3">
       <c r="A40" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="C41" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="C42" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:3">
       <c r="A44" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="C44" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:3">
       <c r="A46" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="C46" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="C47" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:3">
       <c r="A49" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:3">
       <c r="A50" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:3">
       <c r="A51" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="C51" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:3">
       <c r="A53" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="C53" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="C55" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:3">
       <c r="A57" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="C57" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:3">
       <c r="A59" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="C59" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="C61" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:3">
       <c r="A63" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="C63" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:3">
       <c r="A65" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="C65" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="C67" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:3">
       <c r="A69" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="C69" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:3">
       <c r="A71" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="C71" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="C73" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:3">
       <c r="A75" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="C75" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:3">
       <c r="A77" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="C77" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="C79" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:3">
       <c r="A81" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="C81" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:3">
       <c r="A83" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="C83" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:3">
       <c r="A85" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="C85" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:3">
       <c r="A87" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:3">
       <c r="A88" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:3">
       <c r="A89" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:3">
       <c r="A90" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:3">
       <c r="A92" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:3">
       <c r="A93" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:3">
       <c r="A94" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:3">
       <c r="A95" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:3">
       <c r="A96" s="5" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Sun May  3 07:57:40 IST 2020
</commit_message>
<xml_diff>
--- a/output/reports/03-parsed-network-configs.xlsx
+++ b/output/reports/03-parsed-network-configs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="322">
   <si>
     <t>TCL NETWORK ASSESSMENT - [M3] WAN NETWORK DEVICE CONFIGURATION PARSER MODULE</t>
   </si>
@@ -566,6 +566,405 @@
   </si>
   <si>
     <t>ip prefix-list no-default-route seq 10 permit 0.0.0.0/0 ge 1</t>
+  </si>
+  <si>
+    <t>Access-List</t>
+  </si>
+  <si>
+    <t>ip as-path access-list 100 permit _4755_</t>
+  </si>
+  <si>
+    <t>ip access-list standard TATA-MONITORING-SNMP</t>
+  </si>
+  <si>
+    <t>permit 121.244.180.49</t>
+  </si>
+  <si>
+    <t>permit 121.244.180.47</t>
+  </si>
+  <si>
+    <t>permit 121.244.180.37</t>
+  </si>
+  <si>
+    <t>permit 121.244.227.114</t>
+  </si>
+  <si>
+    <t>permit 121.244.180.36</t>
+  </si>
+  <si>
+    <t>permit 121.244.227.113</t>
+  </si>
+  <si>
+    <t>permit 115.114.226.164</t>
+  </si>
+  <si>
+    <t>permit 115.114.9.67</t>
+  </si>
+  <si>
+    <t>permit 115.114.9.68</t>
+  </si>
+  <si>
+    <t>permit 14.143.102.157</t>
+  </si>
+  <si>
+    <t>permit 14.143.102.156</t>
+  </si>
+  <si>
+    <t>permit 14.143.102.155</t>
+  </si>
+  <si>
+    <t>permit 115.110.215.75</t>
+  </si>
+  <si>
+    <t>permit 10.70.0.202</t>
+  </si>
+  <si>
+    <t>permit 115.110.215.76</t>
+  </si>
+  <si>
+    <t>permit 115.110.215.77</t>
+  </si>
+  <si>
+    <t>permit 10.70.0.199</t>
+  </si>
+  <si>
+    <t>permit 202.54.29.81</t>
+  </si>
+  <si>
+    <t>permit 172.31.6.123</t>
+  </si>
+  <si>
+    <t>permit 115.114.146.71</t>
+  </si>
+  <si>
+    <t>permit 115.114.146.70</t>
+  </si>
+  <si>
+    <t>permit 115.114.146.69</t>
+  </si>
+  <si>
+    <t>permit 202.54.29.25</t>
+  </si>
+  <si>
+    <t>permit 115.114.219.35</t>
+  </si>
+  <si>
+    <t>permit 202.54.29.27</t>
+  </si>
+  <si>
+    <t>permit 10.209.19.0 0.0.0.255</t>
+  </si>
+  <si>
+    <t>permit 115.114.226.160 0.0.0.31</t>
+  </si>
+  <si>
+    <t>permit 115.114.219.32 0.0.0.15</t>
+  </si>
+  <si>
+    <t>deny   any</t>
+  </si>
+  <si>
+    <t>ip access-list standard snmpaccess</t>
+  </si>
+  <si>
+    <t>permit 10.4.102.106</t>
+  </si>
+  <si>
+    <t>permit 10.25.145.134</t>
+  </si>
+  <si>
+    <t>permit 10.3.194.217</t>
+  </si>
+  <si>
+    <t>permit 10.3.194.216</t>
+  </si>
+  <si>
+    <t>permit 10.224.196.10</t>
+  </si>
+  <si>
+    <t>permit 10.224.196.11</t>
+  </si>
+  <si>
+    <t>permit 10.224.199.29</t>
+  </si>
+  <si>
+    <t>permit 10.224.199.27</t>
+  </si>
+  <si>
+    <t>permit 10.224.199.26</t>
+  </si>
+  <si>
+    <t>permit 10.25.144.186</t>
+  </si>
+  <si>
+    <t>permit 10.25.144.195</t>
+  </si>
+  <si>
+    <t>permit 10.4.4.91</t>
+  </si>
+  <si>
+    <t>permit 10.4.4.94</t>
+  </si>
+  <si>
+    <t>permit 10.4.4.93</t>
+  </si>
+  <si>
+    <t>permit 10.4.4.83</t>
+  </si>
+  <si>
+    <t>permit 10.4.4.84</t>
+  </si>
+  <si>
+    <t>permit 10.35.41.95</t>
+  </si>
+  <si>
+    <t>permit 10.187.51.224</t>
+  </si>
+  <si>
+    <t>permit 10.187.51.225</t>
+  </si>
+  <si>
+    <t>permit 10.3.165.220</t>
+  </si>
+  <si>
+    <t>permit 10.3.188.49</t>
+  </si>
+  <si>
+    <t>permit 10.4.102.238</t>
+  </si>
+  <si>
+    <t>permit 10.3.168.43</t>
+  </si>
+  <si>
+    <t>permit 10.25.144.18</t>
+  </si>
+  <si>
+    <t>permit 10.3.169.52</t>
+  </si>
+  <si>
+    <t>permit 10.4.12.150</t>
+  </si>
+  <si>
+    <t>permit 10.3.4.152</t>
+  </si>
+  <si>
+    <t>permit 10.3.169.53</t>
+  </si>
+  <si>
+    <t>permit 10.3.169.54</t>
+  </si>
+  <si>
+    <t>permit 10.3.165.50</t>
+  </si>
+  <si>
+    <t>permit 10.8.141.47</t>
+  </si>
+  <si>
+    <t>permit 10.0.12.164</t>
+  </si>
+  <si>
+    <t>permit 10.11.132.38</t>
+  </si>
+  <si>
+    <t>permit 10.3.12.166</t>
+  </si>
+  <si>
+    <t>permit 10.0.12.162</t>
+  </si>
+  <si>
+    <t>permit 10.0.12.163</t>
+  </si>
+  <si>
+    <t>permit 10.0.12.161</t>
+  </si>
+  <si>
+    <t>permit 10.3.128.32</t>
+  </si>
+  <si>
+    <t>permit 10.0.12.170</t>
+  </si>
+  <si>
+    <t>permit 10.0.12.182</t>
+  </si>
+  <si>
+    <t>permit 10.187.50.52</t>
+  </si>
+  <si>
+    <t>permit 10.25.144.61</t>
+  </si>
+  <si>
+    <t>permit 10.187.51.67</t>
+  </si>
+  <si>
+    <t>permit 10.187.51.65</t>
+  </si>
+  <si>
+    <t>permit 10.118.41.147</t>
+  </si>
+  <si>
+    <t>permit 10.3.6.193</t>
+  </si>
+  <si>
+    <t>permit 10.118.41.155</t>
+  </si>
+  <si>
+    <t>permit 10.3.182.106</t>
+  </si>
+  <si>
+    <t>permit 10.4.102.191</t>
+  </si>
+  <si>
+    <t>permit 10.3.149.65</t>
+  </si>
+  <si>
+    <t>permit 10.21.240.48</t>
+  </si>
+  <si>
+    <t>permit 10.187.51.102</t>
+  </si>
+  <si>
+    <t>permit 10.3.169.69</t>
+  </si>
+  <si>
+    <t>permit 10.187.51.101</t>
+  </si>
+  <si>
+    <t>permit 10.187.50.123</t>
+  </si>
+  <si>
+    <t>permit 10.21.240.18</t>
+  </si>
+  <si>
+    <t>permit 10.3.221.0 0.0.0.255</t>
+  </si>
+  <si>
+    <t>permit 10.187.108.0 0.0.0.255</t>
+  </si>
+  <si>
+    <t>permit 10.224.2.0 0.0.0.255</t>
+  </si>
+  <si>
+    <t>ip access-list extended FULLMESH_DENY_LOCAL</t>
+  </si>
+  <si>
+    <t>deny   ip 10.95.22.92 0.0.0.3 any</t>
+  </si>
+  <si>
+    <t>deny   ip any 10.95.22.92 0.0.0.3</t>
+  </si>
+  <si>
+    <t>deny   ip host 172.23.33.41 any</t>
+  </si>
+  <si>
+    <t>deny   ip any host 172.23.33.41</t>
+  </si>
+  <si>
+    <t>deny   ip host 172.23.32.11 any</t>
+  </si>
+  <si>
+    <t>deny   ip any host 172.23.32.11</t>
+  </si>
+  <si>
+    <t>ip access-list extended HUBSPOKE_DENY_LOCAL</t>
+  </si>
+  <si>
+    <t>deny   ip 10.95.25.172 0.0.0.3 any</t>
+  </si>
+  <si>
+    <t>deny   ip any 10.95.25.172 0.0.0.3</t>
+  </si>
+  <si>
+    <t>deny   ip host 172.23.35.92 any</t>
+  </si>
+  <si>
+    <t>deny   ip any host 172.23.35.92</t>
+  </si>
+  <si>
+    <t>ip access-list extended NC1_LAN_BUSINESS.ACL</t>
+  </si>
+  <si>
+    <t>remark *** Class Business ***</t>
+  </si>
+  <si>
+    <t>permit tcp any any range 3200 3399</t>
+  </si>
+  <si>
+    <t>permit tcp any any range 3600 3699</t>
+  </si>
+  <si>
+    <t>permit tcp any range 3200 3399 any</t>
+  </si>
+  <si>
+    <t>permit tcp any range 3600 3699 any</t>
+  </si>
+  <si>
+    <t>permit tcp any any eq 1494</t>
+  </si>
+  <si>
+    <t>permit tcp any eq 1494 any</t>
+  </si>
+  <si>
+    <t>permit tcp any any eq 2598</t>
+  </si>
+  <si>
+    <t>permit tcp any eq 2598 any</t>
+  </si>
+  <si>
+    <t>permit tcp any any eq 1812</t>
+  </si>
+  <si>
+    <t>permit tcp any any eq 1813</t>
+  </si>
+  <si>
+    <t>permit tcp any eq 1812 any</t>
+  </si>
+  <si>
+    <t>permit tcp any eq 1813 any</t>
+  </si>
+  <si>
+    <t>permit tcp any eq 2065 any</t>
+  </si>
+  <si>
+    <t>permit tcp any eq 1996 any</t>
+  </si>
+  <si>
+    <t>permit tcp any any eq 2065</t>
+  </si>
+  <si>
+    <t>permit tcp any any eq 1996</t>
+  </si>
+  <si>
+    <t>permit tcp any any dscp af32</t>
+  </si>
+  <si>
+    <t>deny   ip any any</t>
+  </si>
+  <si>
+    <t>access-list 1 deny   14.0.0.0 0.0.0.3</t>
+  </si>
+  <si>
+    <t>access-list 1 deny   115.0.0.0 0.0.0.15</t>
+  </si>
+  <si>
+    <t>access-list 1 deny   121.0.0.0 0.255.255.255</t>
+  </si>
+  <si>
+    <t>access-list 1 permit any</t>
+  </si>
+  <si>
+    <t>access-list 10 permit 121.244.227.113</t>
+  </si>
+  <si>
+    <t>access-list 10 permit 172.31.6.123</t>
+  </si>
+  <si>
+    <t>access-list 10 permit 202.54.29.25</t>
+  </si>
+  <si>
+    <t>access-list 10 permit 10.209.19.0 0.0.0.255</t>
+  </si>
+  <si>
+    <t>access-list 10 deny   any</t>
   </si>
   <si>
     <t>192.168.0.109</t>
@@ -1058,10 +1457,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>182</v>
+        <v>315</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>183</v>
+        <v>316</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
@@ -1073,7 +1472,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>184</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1081,10 +1480,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>186</v>
+        <v>319</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>187</v>
+        <v>320</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
@@ -1133,7 +1532,7 @@
   <sheetPr>
     <tabColor rgb="FF008000"/>
   </sheetPr>
-  <dimension ref="A2:U218"/>
+  <dimension ref="A2:U238"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1758,12 +2157,20 @@
       <c r="A89" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="C89" s="2" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="5" t="s">
         <v>72</v>
       </c>
     </row>
+    <row r="91" spans="1:3">
+      <c r="C91" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
     <row r="92" spans="1:3">
       <c r="A92" s="5" t="s">
         <v>73</v>
@@ -1773,525 +2180,986 @@
       <c r="A93" s="5" t="s">
         <v>74</v>
       </c>
+      <c r="C93" s="5" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="5" t="s">
         <v>75</v>
       </c>
+      <c r="C94" s="5" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="5" t="s">
         <v>76</v>
       </c>
+      <c r="C95" s="5" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="C96" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="C97" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="C98" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="C99" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="C100" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
+      <c r="C101" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="103" spans="1:1">
+      <c r="C102" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="104" spans="1:1">
+      <c r="C103" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="105" spans="1:1">
+      <c r="C104" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="106" spans="1:1">
+      <c r="C105" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="107" spans="1:1">
+      <c r="C106" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="108" spans="1:1">
+      <c r="C107" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="109" spans="1:1">
+      <c r="C108" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="110" spans="1:1">
+      <c r="C109" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="111" spans="1:1">
+      <c r="C110" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
       <c r="A111" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="C111" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="C112" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
       <c r="A113" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="C113" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="C114" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
       <c r="A115" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="116" spans="1:1">
+      <c r="C115" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
       <c r="A116" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="117" spans="1:1">
+      <c r="C116" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
       <c r="A117" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="118" spans="1:1">
+      <c r="C117" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
       <c r="A118" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="C118" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
       <c r="A119" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="120" spans="1:1">
+      <c r="C119" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
       <c r="A120" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="121" spans="1:1">
+      <c r="C120" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
       <c r="A121" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="122" spans="1:1">
+      <c r="C121" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
       <c r="A122" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="123" spans="1:1">
+      <c r="C122" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
       <c r="A123" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:3">
       <c r="A124" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="125" spans="1:1">
+      <c r="C124" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
       <c r="A125" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="127" spans="1:1">
+      <c r="C125" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="C126" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
       <c r="A127" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="128" spans="1:1">
+      <c r="C127" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
       <c r="A128" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="129" spans="1:1">
+      <c r="C128" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
       <c r="A129" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="130" spans="1:1">
+      <c r="C129" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
       <c r="A130" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="131" spans="1:1">
+      <c r="C130" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
       <c r="A131" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
+      <c r="C131" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
       <c r="A132" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="133" spans="1:1">
+      <c r="C132" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
       <c r="A133" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="134" spans="1:1">
+      <c r="C133" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
       <c r="A134" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="135" spans="1:1">
+      <c r="C134" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
       <c r="A135" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="136" spans="1:1">
+      <c r="C135" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
       <c r="A136" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="137" spans="1:1">
+      <c r="C136" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
       <c r="A137" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="138" spans="1:1">
+      <c r="C137" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
       <c r="A138" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="139" spans="1:1">
+      <c r="C138" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
       <c r="A139" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="143" spans="1:1">
+      <c r="C139" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="C140" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="C141" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="C142" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
       <c r="A143" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="145" spans="1:1">
+      <c r="C143" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="C144" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
       <c r="A145" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="146" spans="1:1">
+      <c r="C145" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
       <c r="A146" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="147" spans="1:1">
+      <c r="C146" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
       <c r="A147" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="149" spans="1:1">
+      <c r="C147" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="C148" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
       <c r="A149" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="150" spans="1:1">
+      <c r="C149" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
       <c r="A150" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="151" spans="1:1">
+      <c r="C150" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
       <c r="A151" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="152" spans="1:1">
+      <c r="C151" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
       <c r="A152" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="154" spans="1:1">
+      <c r="C152" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="C153" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
       <c r="A154" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="155" spans="1:1">
+      <c r="C154" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
       <c r="A155" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="156" spans="1:1">
+      <c r="C155" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
       <c r="A156" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="157" spans="1:1">
+      <c r="C156" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
       <c r="A157" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="159" spans="1:1">
+      <c r="C157" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="C158" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
       <c r="A159" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="160" spans="1:1">
+      <c r="C159" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
       <c r="A160" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="161" spans="1:1">
+      <c r="C160" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
       <c r="A161" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="162" spans="1:1">
+      <c r="C161" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
       <c r="A162" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="164" spans="1:1">
+      <c r="C162" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="C163" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
       <c r="A164" s="5" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="165" spans="1:1">
+      <c r="C164" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
       <c r="A165" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="166" spans="1:1">
+      <c r="C165" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
       <c r="A166" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="167" spans="1:1">
+      <c r="C166" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
       <c r="A167" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="169" spans="1:1">
+      <c r="C167" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="C168" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
       <c r="A169" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="170" spans="1:1">
+      <c r="C169" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
       <c r="A170" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="171" spans="1:1">
+      <c r="C170" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
       <c r="A171" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="172" spans="1:1">
+      <c r="C171" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
       <c r="A172" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="174" spans="1:1">
+      <c r="C172" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="C173" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
       <c r="A174" s="5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="175" spans="1:1">
+      <c r="C174" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
       <c r="A175" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="176" spans="1:1">
+      <c r="C175" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
       <c r="A176" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="177" spans="1:1">
+      <c r="C176" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
       <c r="A177" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="179" spans="1:1">
+      <c r="C177" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="C178" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
       <c r="A179" s="5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="180" spans="1:1">
+      <c r="C179" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
       <c r="A180" s="5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="181" spans="1:1">
+      <c r="C180" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
       <c r="A181" s="5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="182" spans="1:1">
+      <c r="C181" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
       <c r="A182" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="183" spans="1:1">
+      <c r="C182" s="5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
       <c r="A183" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="185" spans="1:1">
+      <c r="C183" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
       <c r="A185" s="5" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="186" spans="1:1">
+      <c r="C185" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
       <c r="A186" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="187" spans="1:1">
+      <c r="C186" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
       <c r="A187" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="188" spans="1:1">
+      <c r="C187" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
       <c r="A188" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="190" spans="1:1">
+      <c r="C188" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="C189" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
       <c r="A190" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="191" spans="1:1">
+      <c r="C190" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
       <c r="A191" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="192" spans="1:1">
+      <c r="C191" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
       <c r="A192" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="194" spans="1:1">
+    <row r="193" spans="1:3">
+      <c r="C193" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
       <c r="A194" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="195" spans="1:1">
+      <c r="C194" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
       <c r="A195" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="196" spans="1:1">
+      <c r="C195" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
       <c r="A196" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="197" spans="1:1">
+      <c r="C196" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
       <c r="A197" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="199" spans="1:1">
+      <c r="C197" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="C198" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
       <c r="A199" s="5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="200" spans="1:1">
+      <c r="C199" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
       <c r="A200" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:3">
       <c r="A201" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="202" spans="1:1">
+      <c r="C201" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
       <c r="A202" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="204" spans="1:1">
+      <c r="C202" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="C203" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
       <c r="A204" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="205" spans="1:1">
+      <c r="C204" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
       <c r="A205" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="206" spans="1:1">
+      <c r="C205" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
       <c r="A206" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="207" spans="1:1">
+      <c r="C206" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
       <c r="A207" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="209" spans="1:1">
+      <c r="C207" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="C208" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
       <c r="A209" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="210" spans="1:1">
+      <c r="C209" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
       <c r="A210" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="211" spans="1:1">
+      <c r="C210" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
       <c r="A211" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="212" spans="1:1">
+      <c r="C211" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
       <c r="A212" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="214" spans="1:1">
+      <c r="C212" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="C213" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
       <c r="A214" s="5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="215" spans="1:1">
+      <c r="C214" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
       <c r="A215" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="216" spans="1:1">
+      <c r="C215" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
       <c r="A216" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="217" spans="1:1">
+      <c r="C216" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
       <c r="A217" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="218" spans="1:1">
+      <c r="C217" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
       <c r="A218" s="5" t="s">
         <v>99</v>
+      </c>
+      <c r="C218" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="C219" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="C220" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="C222" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="C224" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="226" spans="3:3">
+      <c r="C226" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="228" spans="3:3">
+      <c r="C228" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="230" spans="3:3">
+      <c r="C230" s="5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="232" spans="3:3">
+      <c r="C232" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="234" spans="3:3">
+      <c r="C234" s="5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="236" spans="3:3">
+      <c r="C236" s="5" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="238" spans="3:3">
+      <c r="C238" s="5" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2310,7 +3178,7 @@
   <sheetPr>
     <tabColor rgb="FF008000"/>
   </sheetPr>
-  <dimension ref="A2:U218"/>
+  <dimension ref="A2:U238"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2329,7 +3197,7 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>185</v>
+        <v>318</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2935,12 +3803,20 @@
       <c r="A89" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="C89" s="2" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="5" t="s">
         <v>72</v>
       </c>
     </row>
+    <row r="91" spans="1:3">
+      <c r="C91" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
     <row r="92" spans="1:3">
       <c r="A92" s="5" t="s">
         <v>73</v>
@@ -2950,525 +3826,986 @@
       <c r="A93" s="5" t="s">
         <v>74</v>
       </c>
+      <c r="C93" s="5" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="5" t="s">
         <v>75</v>
       </c>
+      <c r="C94" s="5" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="5" t="s">
         <v>76</v>
       </c>
+      <c r="C95" s="5" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="C96" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="C97" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="C98" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="C99" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="C100" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
+      <c r="C101" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="103" spans="1:1">
+      <c r="C102" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="104" spans="1:1">
+      <c r="C103" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="105" spans="1:1">
+      <c r="C104" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="106" spans="1:1">
+      <c r="C105" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="107" spans="1:1">
+      <c r="C106" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="108" spans="1:1">
+      <c r="C107" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="109" spans="1:1">
+      <c r="C108" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="110" spans="1:1">
+      <c r="C109" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="111" spans="1:1">
+      <c r="C110" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
       <c r="A111" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="C111" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="C112" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
       <c r="A113" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="C113" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="C114" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
       <c r="A115" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="116" spans="1:1">
+      <c r="C115" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
       <c r="A116" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="117" spans="1:1">
+      <c r="C116" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
       <c r="A117" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="118" spans="1:1">
+      <c r="C117" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
       <c r="A118" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="C118" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
       <c r="A119" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="120" spans="1:1">
+      <c r="C119" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
       <c r="A120" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="121" spans="1:1">
+      <c r="C120" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
       <c r="A121" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="122" spans="1:1">
+      <c r="C121" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
       <c r="A122" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="123" spans="1:1">
+      <c r="C122" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
       <c r="A123" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:3">
       <c r="A124" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="125" spans="1:1">
+      <c r="C124" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
       <c r="A125" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="127" spans="1:1">
+      <c r="C125" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="C126" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
       <c r="A127" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="128" spans="1:1">
+      <c r="C127" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
       <c r="A128" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="129" spans="1:1">
+      <c r="C128" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
       <c r="A129" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="130" spans="1:1">
+      <c r="C129" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
       <c r="A130" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="131" spans="1:1">
+      <c r="C130" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
       <c r="A131" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
+      <c r="C131" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
       <c r="A132" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="133" spans="1:1">
+      <c r="C132" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
       <c r="A133" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="134" spans="1:1">
+      <c r="C133" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
       <c r="A134" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="135" spans="1:1">
+      <c r="C134" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
       <c r="A135" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="136" spans="1:1">
+      <c r="C135" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
       <c r="A136" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="137" spans="1:1">
+      <c r="C136" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
       <c r="A137" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="138" spans="1:1">
+      <c r="C137" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
       <c r="A138" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="139" spans="1:1">
+      <c r="C138" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
       <c r="A139" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="143" spans="1:1">
+      <c r="C139" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="C140" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="C141" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="C142" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
       <c r="A143" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="145" spans="1:1">
+      <c r="C143" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="C144" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
       <c r="A145" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="146" spans="1:1">
+      <c r="C145" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
       <c r="A146" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="147" spans="1:1">
+      <c r="C146" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
       <c r="A147" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="149" spans="1:1">
+      <c r="C147" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="C148" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
       <c r="A149" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="150" spans="1:1">
+      <c r="C149" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
       <c r="A150" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="151" spans="1:1">
+      <c r="C150" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
       <c r="A151" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="152" spans="1:1">
+      <c r="C151" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
       <c r="A152" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="154" spans="1:1">
+      <c r="C152" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="C153" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
       <c r="A154" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="155" spans="1:1">
+      <c r="C154" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
       <c r="A155" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="156" spans="1:1">
+      <c r="C155" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
       <c r="A156" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="157" spans="1:1">
+      <c r="C156" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
       <c r="A157" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="159" spans="1:1">
+      <c r="C157" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="C158" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
       <c r="A159" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="160" spans="1:1">
+      <c r="C159" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
       <c r="A160" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="161" spans="1:1">
+      <c r="C160" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
       <c r="A161" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="162" spans="1:1">
+      <c r="C161" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
       <c r="A162" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="164" spans="1:1">
+      <c r="C162" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="C163" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
       <c r="A164" s="5" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="165" spans="1:1">
+      <c r="C164" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
       <c r="A165" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="166" spans="1:1">
+      <c r="C165" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
       <c r="A166" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="167" spans="1:1">
+      <c r="C166" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
       <c r="A167" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="169" spans="1:1">
+      <c r="C167" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="C168" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
       <c r="A169" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="170" spans="1:1">
+      <c r="C169" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
       <c r="A170" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="171" spans="1:1">
+      <c r="C170" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
       <c r="A171" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="172" spans="1:1">
+      <c r="C171" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
       <c r="A172" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="174" spans="1:1">
+      <c r="C172" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="C173" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
       <c r="A174" s="5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="175" spans="1:1">
+      <c r="C174" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
       <c r="A175" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="176" spans="1:1">
+      <c r="C175" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
       <c r="A176" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="177" spans="1:1">
+      <c r="C176" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
       <c r="A177" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="179" spans="1:1">
+      <c r="C177" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="C178" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
       <c r="A179" s="5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="180" spans="1:1">
+      <c r="C179" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
       <c r="A180" s="5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="181" spans="1:1">
+      <c r="C180" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
       <c r="A181" s="5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="182" spans="1:1">
+      <c r="C181" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
       <c r="A182" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="183" spans="1:1">
+      <c r="C182" s="5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
       <c r="A183" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="185" spans="1:1">
+      <c r="C183" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
       <c r="A185" s="5" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="186" spans="1:1">
+      <c r="C185" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
       <c r="A186" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="187" spans="1:1">
+      <c r="C186" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
       <c r="A187" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="188" spans="1:1">
+      <c r="C187" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
       <c r="A188" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="190" spans="1:1">
+      <c r="C188" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="C189" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
       <c r="A190" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="191" spans="1:1">
+      <c r="C190" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
       <c r="A191" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="192" spans="1:1">
+      <c r="C191" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
       <c r="A192" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="194" spans="1:1">
+    <row r="193" spans="1:3">
+      <c r="C193" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
       <c r="A194" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="195" spans="1:1">
+      <c r="C194" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
       <c r="A195" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="196" spans="1:1">
+      <c r="C195" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
       <c r="A196" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="197" spans="1:1">
+      <c r="C196" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
       <c r="A197" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="199" spans="1:1">
+      <c r="C197" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="C198" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
       <c r="A199" s="5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="200" spans="1:1">
+      <c r="C199" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
       <c r="A200" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:3">
       <c r="A201" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="202" spans="1:1">
+      <c r="C201" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
       <c r="A202" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="204" spans="1:1">
+      <c r="C202" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="C203" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
       <c r="A204" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="205" spans="1:1">
+      <c r="C204" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
       <c r="A205" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="206" spans="1:1">
+      <c r="C205" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
       <c r="A206" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="207" spans="1:1">
+      <c r="C206" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
       <c r="A207" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="209" spans="1:1">
+      <c r="C207" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="C208" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
       <c r="A209" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="210" spans="1:1">
+      <c r="C209" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
       <c r="A210" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="211" spans="1:1">
+      <c r="C210" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
       <c r="A211" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="212" spans="1:1">
+      <c r="C211" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
       <c r="A212" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="214" spans="1:1">
+      <c r="C212" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="C213" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
       <c r="A214" s="5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="215" spans="1:1">
+      <c r="C214" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
       <c r="A215" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="216" spans="1:1">
+      <c r="C215" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
       <c r="A216" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="217" spans="1:1">
+      <c r="C216" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
       <c r="A217" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="218" spans="1:1">
+      <c r="C217" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
       <c r="A218" s="5" t="s">
         <v>99</v>
+      </c>
+      <c r="C218" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="C219" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="C220" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="C222" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="C224" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="226" spans="3:3">
+      <c r="C226" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="228" spans="3:3">
+      <c r="C228" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="230" spans="3:3">
+      <c r="C230" s="5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="232" spans="3:3">
+      <c r="C232" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="234" spans="3:3">
+      <c r="C234" s="5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="236" spans="3:3">
+      <c r="C236" s="5" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="238" spans="3:3">
+      <c r="C238" s="5" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -3487,7 +4824,7 @@
   <sheetPr>
     <tabColor rgb="FF008000"/>
   </sheetPr>
-  <dimension ref="A2:U218"/>
+  <dimension ref="A2:U238"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3506,7 +4843,7 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>188</v>
+        <v>321</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4112,12 +5449,20 @@
       <c r="A89" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="C89" s="2" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="5" t="s">
         <v>72</v>
       </c>
     </row>
+    <row r="91" spans="1:3">
+      <c r="C91" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
     <row r="92" spans="1:3">
       <c r="A92" s="5" t="s">
         <v>73</v>
@@ -4127,525 +5472,986 @@
       <c r="A93" s="5" t="s">
         <v>74</v>
       </c>
+      <c r="C93" s="5" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="5" t="s">
         <v>75</v>
       </c>
+      <c r="C94" s="5" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="5" t="s">
         <v>76</v>
       </c>
+      <c r="C95" s="5" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="C96" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="C97" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="C98" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="C99" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="C100" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
+      <c r="C101" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="103" spans="1:1">
+      <c r="C102" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="104" spans="1:1">
+      <c r="C103" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="105" spans="1:1">
+      <c r="C104" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="106" spans="1:1">
+      <c r="C105" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="107" spans="1:1">
+      <c r="C106" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="108" spans="1:1">
+      <c r="C107" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="109" spans="1:1">
+      <c r="C108" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="110" spans="1:1">
+      <c r="C109" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="111" spans="1:1">
+      <c r="C110" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
       <c r="A111" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="C111" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="C112" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
       <c r="A113" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="C113" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="C114" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
       <c r="A115" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="116" spans="1:1">
+      <c r="C115" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
       <c r="A116" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="117" spans="1:1">
+      <c r="C116" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
       <c r="A117" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="118" spans="1:1">
+      <c r="C117" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
       <c r="A118" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="C118" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
       <c r="A119" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="120" spans="1:1">
+      <c r="C119" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
       <c r="A120" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="121" spans="1:1">
+      <c r="C120" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
       <c r="A121" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="122" spans="1:1">
+      <c r="C121" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
       <c r="A122" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="123" spans="1:1">
+      <c r="C122" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
       <c r="A123" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:3">
       <c r="A124" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="125" spans="1:1">
+      <c r="C124" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
       <c r="A125" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="127" spans="1:1">
+      <c r="C125" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="C126" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
       <c r="A127" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="128" spans="1:1">
+      <c r="C127" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
       <c r="A128" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="129" spans="1:1">
+      <c r="C128" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
       <c r="A129" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="130" spans="1:1">
+      <c r="C129" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
       <c r="A130" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="131" spans="1:1">
+      <c r="C130" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
       <c r="A131" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
+      <c r="C131" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
       <c r="A132" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="133" spans="1:1">
+      <c r="C132" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
       <c r="A133" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="134" spans="1:1">
+      <c r="C133" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
       <c r="A134" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="135" spans="1:1">
+      <c r="C134" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
       <c r="A135" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="136" spans="1:1">
+      <c r="C135" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
       <c r="A136" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="137" spans="1:1">
+      <c r="C136" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
       <c r="A137" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="138" spans="1:1">
+      <c r="C137" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
       <c r="A138" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="139" spans="1:1">
+      <c r="C138" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
       <c r="A139" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="143" spans="1:1">
+      <c r="C139" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="C140" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="C141" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="C142" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
       <c r="A143" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="145" spans="1:1">
+      <c r="C143" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="C144" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
       <c r="A145" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="146" spans="1:1">
+      <c r="C145" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
       <c r="A146" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="147" spans="1:1">
+      <c r="C146" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
       <c r="A147" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="149" spans="1:1">
+      <c r="C147" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="C148" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
       <c r="A149" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="150" spans="1:1">
+      <c r="C149" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
       <c r="A150" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="151" spans="1:1">
+      <c r="C150" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
       <c r="A151" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="152" spans="1:1">
+      <c r="C151" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
       <c r="A152" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="154" spans="1:1">
+      <c r="C152" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="C153" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
       <c r="A154" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="155" spans="1:1">
+      <c r="C154" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
       <c r="A155" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="156" spans="1:1">
+      <c r="C155" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
       <c r="A156" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="157" spans="1:1">
+      <c r="C156" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
       <c r="A157" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="159" spans="1:1">
+      <c r="C157" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="C158" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
       <c r="A159" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="160" spans="1:1">
+      <c r="C159" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
       <c r="A160" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="161" spans="1:1">
+      <c r="C160" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
       <c r="A161" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="162" spans="1:1">
+      <c r="C161" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
       <c r="A162" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="164" spans="1:1">
+      <c r="C162" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="C163" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
       <c r="A164" s="5" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="165" spans="1:1">
+      <c r="C164" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
       <c r="A165" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="166" spans="1:1">
+      <c r="C165" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
       <c r="A166" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="167" spans="1:1">
+      <c r="C166" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
       <c r="A167" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="169" spans="1:1">
+      <c r="C167" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="C168" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
       <c r="A169" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="170" spans="1:1">
+      <c r="C169" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
       <c r="A170" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="171" spans="1:1">
+      <c r="C170" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
       <c r="A171" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="172" spans="1:1">
+      <c r="C171" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
       <c r="A172" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="174" spans="1:1">
+      <c r="C172" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="C173" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
       <c r="A174" s="5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="175" spans="1:1">
+      <c r="C174" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
       <c r="A175" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="176" spans="1:1">
+      <c r="C175" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
       <c r="A176" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="177" spans="1:1">
+      <c r="C176" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
       <c r="A177" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="179" spans="1:1">
+      <c r="C177" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="C178" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
       <c r="A179" s="5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="180" spans="1:1">
+      <c r="C179" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
       <c r="A180" s="5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="181" spans="1:1">
+      <c r="C180" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
       <c r="A181" s="5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="182" spans="1:1">
+      <c r="C181" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
       <c r="A182" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="183" spans="1:1">
+      <c r="C182" s="5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
       <c r="A183" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="185" spans="1:1">
+      <c r="C183" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
       <c r="A185" s="5" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="186" spans="1:1">
+      <c r="C185" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
       <c r="A186" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="187" spans="1:1">
+      <c r="C186" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
       <c r="A187" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="188" spans="1:1">
+      <c r="C187" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
       <c r="A188" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="190" spans="1:1">
+      <c r="C188" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="C189" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
       <c r="A190" s="5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="191" spans="1:1">
+      <c r="C190" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
       <c r="A191" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="192" spans="1:1">
+      <c r="C191" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
       <c r="A192" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="194" spans="1:1">
+    <row r="193" spans="1:3">
+      <c r="C193" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
       <c r="A194" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="195" spans="1:1">
+      <c r="C194" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
       <c r="A195" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="196" spans="1:1">
+      <c r="C195" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
       <c r="A196" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="197" spans="1:1">
+      <c r="C196" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
       <c r="A197" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="199" spans="1:1">
+      <c r="C197" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="C198" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
       <c r="A199" s="5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="200" spans="1:1">
+      <c r="C199" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
       <c r="A200" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:3">
       <c r="A201" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="202" spans="1:1">
+      <c r="C201" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
       <c r="A202" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="204" spans="1:1">
+      <c r="C202" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="C203" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
       <c r="A204" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="205" spans="1:1">
+      <c r="C204" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
       <c r="A205" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="206" spans="1:1">
+      <c r="C205" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
       <c r="A206" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="207" spans="1:1">
+      <c r="C206" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
       <c r="A207" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="209" spans="1:1">
+      <c r="C207" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="C208" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
       <c r="A209" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="210" spans="1:1">
+      <c r="C209" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
       <c r="A210" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="211" spans="1:1">
+      <c r="C210" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
       <c r="A211" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="212" spans="1:1">
+      <c r="C211" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
       <c r="A212" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="214" spans="1:1">
+      <c r="C212" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="C213" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
       <c r="A214" s="5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="215" spans="1:1">
+      <c r="C214" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
       <c r="A215" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="216" spans="1:1">
+      <c r="C215" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
       <c r="A216" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="217" spans="1:1">
+      <c r="C216" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
       <c r="A217" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="218" spans="1:1">
+      <c r="C217" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
       <c r="A218" s="5" t="s">
         <v>99</v>
+      </c>
+      <c r="C218" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="C219" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="C220" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="C222" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="C224" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="226" spans="3:3">
+      <c r="C226" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="228" spans="3:3">
+      <c r="C228" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="230" spans="3:3">
+      <c r="C230" s="5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="232" spans="3:3">
+      <c r="C232" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="234" spans="3:3">
+      <c r="C234" s="5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="236" spans="3:3">
+      <c r="C236" s="5" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="238" spans="3:3">
+      <c r="C238" s="5" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>